<commit_message>
calculados indicadores financieros para RE
</commit_message>
<xml_diff>
--- a/SAP - NEGOCIO/Temporal/Plan ECO FINAN/Plan ECO-FINAN-PUM.xlsx
+++ b/SAP - NEGOCIO/Temporal/Plan ECO FINAN/Plan ECO-FINAN-PUM.xlsx
@@ -9,12 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Ingresos" sheetId="1" r:id="rId1"/>
-    <sheet name="Precios " sheetId="2" r:id="rId2"/>
-    <sheet name="Volumenes" sheetId="3" r:id="rId3"/>
+    <sheet name="Ganancias" sheetId="5" r:id="rId2"/>
+    <sheet name="Costos" sheetId="6" r:id="rId3"/>
+    <sheet name="Indicadores Financieros" sheetId="4" r:id="rId4"/>
+    <sheet name="Precios " sheetId="2" r:id="rId5"/>
+    <sheet name="Volumenes" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
   <si>
     <t>Mes</t>
   </si>
@@ -167,12 +170,76 @@
   <si>
     <t>Semestre 2 - 2017</t>
   </si>
+  <si>
+    <t>año</t>
+  </si>
+  <si>
+    <t>Ingreso</t>
+  </si>
+  <si>
+    <t>Gastos Fijos</t>
+  </si>
+  <si>
+    <t>Gastos Variables</t>
+  </si>
+  <si>
+    <t>Aguinaldos</t>
+  </si>
+  <si>
+    <t>Año 1</t>
+  </si>
+  <si>
+    <t>Año 2</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>Ingresos</t>
+  </si>
+  <si>
+    <t>Egresos</t>
+  </si>
+  <si>
+    <t>Ganancia Neta</t>
+  </si>
+  <si>
+    <t>imp ganancia</t>
+  </si>
+  <si>
+    <t>GANANCIAS</t>
+  </si>
+  <si>
+    <t>TASA</t>
+  </si>
+  <si>
+    <t>VAN</t>
+  </si>
+  <si>
+    <t>TIR</t>
+  </si>
+  <si>
+    <t>cashflow</t>
+  </si>
+  <si>
+    <t>meses</t>
+  </si>
+  <si>
+    <t>3 meses</t>
+  </si>
+  <si>
+    <t>6 dias</t>
+  </si>
+  <si>
+    <t>1 año</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;\ #,##0.00;[Red]&quot;$&quot;\ \-#,##0.00"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
@@ -299,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -342,6 +409,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -650,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,11 +784,11 @@
       </c>
       <c r="E3" s="19">
         <f>(('Precios '!E4*'Precios '!B5)+('Precios '!B6*Volumenes!F4)+('Precios '!B7*Volumenes!G4)+('Precios '!B8*Volumenes!H4))*6</f>
-        <v>333000</v>
+        <v>213000</v>
       </c>
       <c r="F3" s="19">
         <f>SUM(B3:E3)</f>
-        <v>1342000</v>
+        <v>1222000</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -738,11 +809,11 @@
       </c>
       <c r="E4" s="19">
         <f>(('Precios '!E4*'Precios '!B6)+('Precios '!B6*Volumenes!F5)+('Precios '!B7*Volumenes!G5)+('Precios '!B8*Volumenes!H5))*6</f>
-        <v>426000</v>
+        <v>346800</v>
       </c>
       <c r="F4" s="19">
         <f>SUM(B4:E4)</f>
-        <v>1536000</v>
+        <v>1456800</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -751,23 +822,23 @@
       </c>
       <c r="B5" s="8">
         <f>6*Volumenes!B6*'Precios '!B11</f>
-        <v>1587600</v>
+        <v>1146600</v>
       </c>
       <c r="C5" s="8">
         <f>'Precios '!B12*Volumenes!C6*6</f>
-        <v>1260000</v>
+        <v>882000</v>
       </c>
       <c r="D5" s="8">
         <f>'Precios '!B13*Volumenes!D6</f>
-        <v>70000</v>
+        <v>56000</v>
       </c>
       <c r="E5" s="8">
         <f>(('Precios '!B14*Volumenes!E6)+('Precios '!B15*Volumenes!F6)+('Precios '!B16*Volumenes!G6)+('Precios '!B17*Volumenes!H6))*6</f>
-        <v>1444800</v>
+        <v>473760</v>
       </c>
       <c r="F5" s="9">
         <f>SUM(B5:E5)</f>
-        <v>4362400</v>
+        <v>2558360</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -776,23 +847,47 @@
       </c>
       <c r="B6" s="8">
         <f>6*'Precios '!B11*Volumenes!B7</f>
-        <v>441000</v>
+        <v>1852200</v>
       </c>
       <c r="C6" s="8">
         <f>'Precios '!B12*Volumenes!C7*6</f>
-        <v>3150000</v>
+        <v>1134000</v>
       </c>
       <c r="D6" s="8">
         <f>'Precios '!B13*Volumenes!D7</f>
-        <v>84000</v>
+        <v>28000</v>
       </c>
       <c r="E6" s="8">
         <f>(('Precios '!B14*Volumenes!E7)+('Precios '!B15*Volumenes!F7)+('Precios '!B16*Volumenes!G7)+('Precios '!B17*Volumenes!H7))*6</f>
-        <v>1296120</v>
+        <v>366240</v>
       </c>
       <c r="F6" s="9">
         <f>SUM(B6:E6)</f>
-        <v>4971120</v>
+        <v>3380440</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10">
+        <v>2016</v>
+      </c>
+      <c r="D10">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="24">
+        <f>SUM(F3:F4)</f>
+        <v>2678800</v>
+      </c>
+      <c r="D11" s="24">
+        <f>SUM(F5:F6)</f>
+        <v>5938800</v>
       </c>
     </row>
   </sheetData>
@@ -805,10 +900,320 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2">
+        <f>Ingresos!C11</f>
+        <v>2678800</v>
+      </c>
+      <c r="C2">
+        <f>Ingresos!D11</f>
+        <v>5938800</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3">
+        <f>Costos!B5</f>
+        <v>2629088</v>
+      </c>
+      <c r="C3">
+        <f>Costos!C5</f>
+        <v>4144550</v>
+      </c>
+      <c r="G3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="17">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4">
+        <f>B2-B3</f>
+        <v>49712</v>
+      </c>
+      <c r="C4">
+        <f>C2-C3</f>
+        <v>1794250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5">
+        <f>-(B4*H3)</f>
+        <v>-17399.199999999997</v>
+      </c>
+      <c r="C5">
+        <f>-(C4*H3)</f>
+        <v>-627987.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6">
+        <f>SUM(B4:B5)</f>
+        <v>32312.800000000003</v>
+      </c>
+      <c r="C6">
+        <f>SUM(C4:C5)</f>
+        <v>1166262.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>2086920</v>
+      </c>
+      <c r="C2">
+        <f>B2+(B2*'Precios '!G3)+503577</f>
+        <v>3425265</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>420000</v>
+      </c>
+      <c r="C3">
+        <f>B3+(B3*'Precios '!G4)+128250</f>
+        <v>548250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>122168</v>
+      </c>
+      <c r="C4">
+        <v>171035</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="25">
+        <f>SUM(B2:B4)</f>
+        <v>2629088</v>
+      </c>
+      <c r="C5" s="25">
+        <f>SUM(C2:C4)</f>
+        <v>4144550</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>-342853</v>
+      </c>
+      <c r="C3">
+        <f>Ganancias!B6</f>
+        <v>32312.800000000003</v>
+      </c>
+      <c r="D3">
+        <f>Ganancias!C6</f>
+        <v>1166262.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="27">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="26">
+        <f>NPV(I4,C3:D3)+B3</f>
+        <v>449221.69561768265</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="27">
+        <f>IRR(B3:D3)</f>
+        <v>0.8920788701088187</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14">
+        <f>B3</f>
+        <v>-342853</v>
+      </c>
+      <c r="C14">
+        <f>B14+C3</f>
+        <v>-310540.2</v>
+      </c>
+      <c r="D14">
+        <f>C14+D3</f>
+        <v>855722.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f>D3</f>
+        <v>1166262.5</v>
+      </c>
+      <c r="C17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f>-(C14)</f>
+        <v>310540.2</v>
+      </c>
+      <c r="C18">
+        <f>(B18*C17)/B17</f>
+        <v>3.1952346920183068</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,7 +1290,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="15">
-        <v>2000</v>
+        <v>1700</v>
       </c>
       <c r="C5" s="11">
         <v>2016</v>
@@ -897,7 +1302,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="15">
-        <v>7500</v>
+        <v>6500</v>
       </c>
       <c r="C6" s="11">
         <v>2016</v>
@@ -919,7 +1324,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="15">
-        <v>1600</v>
+        <v>1400</v>
       </c>
       <c r="C8" s="11">
         <v>2016</v>
@@ -983,7 +1388,7 @@
       </c>
       <c r="B14" s="15">
         <f>B5+B5*G3</f>
-        <v>2800</v>
+        <v>2380</v>
       </c>
       <c r="C14" s="11">
         <v>2017</v>
@@ -995,7 +1400,7 @@
       </c>
       <c r="B15" s="15">
         <f>B6+B6*G3</f>
-        <v>10500</v>
+        <v>9100</v>
       </c>
       <c r="C15" s="11">
         <v>2017</v>
@@ -1019,7 +1424,7 @@
       </c>
       <c r="B17" s="15">
         <f>B8+B8*G3</f>
-        <v>2240</v>
+        <v>1960</v>
       </c>
       <c r="C17" s="11">
         <v>2017</v>
@@ -1033,12 +1438,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1120,13 +1525,13 @@
         <v>4</v>
       </c>
       <c r="F4" s="20">
+        <v>4</v>
+      </c>
+      <c r="G4" s="20">
         <v>5</v>
       </c>
-      <c r="G4" s="20">
-        <v>4</v>
-      </c>
       <c r="H4" s="20">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1143,7 +1548,7 @@
         <v>3000</v>
       </c>
       <c r="E5" s="20">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F5" s="20">
         <v>7</v>
@@ -1152,7 +1557,7 @@
         <v>5</v>
       </c>
       <c r="H5" s="20">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1160,25 +1565,25 @@
         <v>30</v>
       </c>
       <c r="B6" s="13">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C6" s="13">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D6" s="6">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="E6" s="6">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="F6" s="6">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G6" s="6">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H6" s="6">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1186,25 +1591,25 @@
         <v>31</v>
       </c>
       <c r="B7" s="13">
+        <v>21</v>
+      </c>
+      <c r="C7" s="13">
+        <v>9</v>
+      </c>
+      <c r="D7" s="6">
+        <v>2000</v>
+      </c>
+      <c r="E7" s="6">
         <v>5</v>
       </c>
-      <c r="C7" s="13">
-        <v>25</v>
-      </c>
-      <c r="D7" s="6">
-        <v>6000</v>
-      </c>
-      <c r="E7" s="6">
-        <v>20</v>
-      </c>
       <c r="F7" s="6">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G7" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H7" s="6">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="I7" s="1"/>
     </row>

</xml_diff>

<commit_message>
modificado van y tir y agregada cadena de valor al gnral
</commit_message>
<xml_diff>
--- a/SAP - NEGOCIO/Temporal/Plan ECO FINAN/Plan ECO-FINAN-PUM.xlsx
+++ b/SAP - NEGOCIO/Temporal/Plan ECO FINAN/Plan ECO-FINAN-PUM.xlsx
@@ -225,13 +225,13 @@
     <t>meses</t>
   </si>
   <si>
-    <t>3 meses</t>
-  </si>
-  <si>
-    <t>6 dias</t>
-  </si>
-  <si>
     <t>1 año</t>
+  </si>
+  <si>
+    <t>se le restó inflacion</t>
+  </si>
+  <si>
+    <t>5 meses</t>
   </si>
 </sst>
 </file>
@@ -400,6 +400,10 @@
     <xf numFmtId="17" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -409,10 +413,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,13 +738,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -881,11 +881,11 @@
       <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="21">
         <f>SUM(F3:F4)</f>
         <v>2678800</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="21">
         <f>SUM(F5:F6)</f>
         <v>5938800</v>
       </c>
@@ -903,7 +903,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,11 +1056,11 @@
       <c r="A5" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="22">
         <f>SUM(B2:B4)</f>
         <v>2629088</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="22">
         <f>SUM(C2:C4)</f>
         <v>4144550</v>
       </c>
@@ -1075,12 +1075,13 @@
   <dimension ref="A2:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1106,15 +1107,18 @@
         <v>32312.800000000003</v>
       </c>
       <c r="D3">
-        <f>Ganancias!C6</f>
-        <v>1166262.5</v>
+        <f>Ganancias!C6-Ganancias!C6*0.4</f>
+        <v>699757.5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H4" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="27">
+      <c r="I4" s="24">
         <v>0.23400000000000001</v>
       </c>
     </row>
@@ -1122,18 +1126,18 @@
       <c r="A9" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9" s="23">
         <f>NPV(I4,C3:D3)+B3</f>
-        <v>449221.69561768265</v>
+        <v>142865.98268665507</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="27">
+      <c r="B10" s="24">
         <f>IRR(B3:D3)</f>
-        <v>0.8920788701088187</v>
+        <v>0.4765305007983307</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1164,7 +1168,7 @@
       </c>
       <c r="D14">
         <f>C14+D3</f>
-        <v>855722.3</v>
+        <v>389217.3</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1172,34 +1176,31 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>D3</f>
-        <v>1166262.5</v>
+        <v>699757.5</v>
       </c>
       <c r="C17">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18">
         <f>-(C14)</f>
         <v>310540.2</v>
       </c>
       <c r="C18">
         <f>(B18*C17)/B17</f>
-        <v>3.1952346920183068</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+        <v>5.3253911533638441</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
         <v>52</v>
-      </c>
-      <c r="C20" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1456,31 +1457,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22" t="s">
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
arreglo de orden de pestañas
</commit_message>
<xml_diff>
--- a/SAP - NEGOCIO/Temporal/Plan ECO FINAN/Plan ECO-FINAN-PUM.xlsx
+++ b/SAP - NEGOCIO/Temporal/Plan ECO FINAN/Plan ECO-FINAN-PUM.xlsx
@@ -12,12 +12,12 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Ingresos" sheetId="1" r:id="rId1"/>
-    <sheet name="Ganancias" sheetId="5" r:id="rId2"/>
-    <sheet name="Costos" sheetId="6" r:id="rId3"/>
-    <sheet name="Indicadores Financieros" sheetId="4" r:id="rId4"/>
-    <sheet name="Precios " sheetId="2" r:id="rId5"/>
-    <sheet name="Volumenes" sheetId="3" r:id="rId6"/>
+    <sheet name="01-Tipo Ingreso" sheetId="2" r:id="rId1"/>
+    <sheet name="02-Volumenes Ingresos" sheetId="3" r:id="rId2"/>
+    <sheet name="03-Ingresos" sheetId="1" r:id="rId3"/>
+    <sheet name="04-Gastos" sheetId="6" r:id="rId4"/>
+    <sheet name="Ganancias" sheetId="5" r:id="rId5"/>
+    <sheet name="Indicadores Financieros" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -326,7 +326,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -362,11 +362,83 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -400,7 +472,6 @@
     <xf numFmtId="17" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -412,6 +483,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -721,496 +802,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-    </row>
-    <row r="2" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="19">
-        <f>6*'Precios '!B2*Volumenes!B4</f>
-        <v>819000</v>
-      </c>
-      <c r="C3" s="19">
-        <f>6*'Precios '!B3*Volumenes!C4</f>
-        <v>180000</v>
-      </c>
-      <c r="D3" s="19">
-        <f>'Precios '!B4*Volumenes!D4</f>
-        <v>10000</v>
-      </c>
-      <c r="E3" s="19">
-        <f>(('Precios '!E4*'Precios '!B5)+('Precios '!B6*Volumenes!F4)+('Precios '!B7*Volumenes!G4)+('Precios '!B8*Volumenes!H4))*6</f>
-        <v>213000</v>
-      </c>
-      <c r="F3" s="19">
-        <f>SUM(B3:E3)</f>
-        <v>1222000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="19">
-        <f>6*'Precios '!B2*Volumenes!B5</f>
-        <v>630000</v>
-      </c>
-      <c r="C4" s="19">
-        <f>6*'Precios '!B3*Volumenes!C5</f>
-        <v>450000</v>
-      </c>
-      <c r="D4" s="19">
-        <f>'Precios '!B4*Volumenes!D5</f>
-        <v>30000</v>
-      </c>
-      <c r="E4" s="19">
-        <f>(('Precios '!E4*'Precios '!B6)+('Precios '!B6*Volumenes!F5)+('Precios '!B7*Volumenes!G5)+('Precios '!B8*Volumenes!H5))*6</f>
-        <v>346800</v>
-      </c>
-      <c r="F4" s="19">
-        <f>SUM(B4:E4)</f>
-        <v>1456800</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="8">
-        <f>6*Volumenes!B6*'Precios '!B11</f>
-        <v>1146600</v>
-      </c>
-      <c r="C5" s="8">
-        <f>'Precios '!B12*Volumenes!C6*6</f>
-        <v>882000</v>
-      </c>
-      <c r="D5" s="8">
-        <f>'Precios '!B13*Volumenes!D6</f>
-        <v>56000</v>
-      </c>
-      <c r="E5" s="8">
-        <f>(('Precios '!B14*Volumenes!E6)+('Precios '!B15*Volumenes!F6)+('Precios '!B16*Volumenes!G6)+('Precios '!B17*Volumenes!H6))*6</f>
-        <v>473760</v>
-      </c>
-      <c r="F5" s="9">
-        <f>SUM(B5:E5)</f>
-        <v>2558360</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="8">
-        <f>6*'Precios '!B11*Volumenes!B7</f>
-        <v>1852200</v>
-      </c>
-      <c r="C6" s="8">
-        <f>'Precios '!B12*Volumenes!C7*6</f>
-        <v>1134000</v>
-      </c>
-      <c r="D6" s="8">
-        <f>'Precios '!B13*Volumenes!D7</f>
-        <v>28000</v>
-      </c>
-      <c r="E6" s="8">
-        <f>(('Precios '!B14*Volumenes!E7)+('Precios '!B15*Volumenes!F7)+('Precios '!B16*Volumenes!G7)+('Precios '!B17*Volumenes!H7))*6</f>
-        <v>366240</v>
-      </c>
-      <c r="F6" s="9">
-        <f>SUM(B6:E6)</f>
-        <v>3380440</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10">
-        <v>2016</v>
-      </c>
-      <c r="D10">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="21">
-        <f>SUM(F3:F4)</f>
-        <v>2678800</v>
-      </c>
-      <c r="D11" s="21">
-        <f>SUM(F5:F6)</f>
-        <v>5938800</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:F1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2">
-        <f>Ingresos!C11</f>
-        <v>2678800</v>
-      </c>
-      <c r="C2">
-        <f>Ingresos!D11</f>
-        <v>5938800</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3">
-        <f>Costos!B5</f>
-        <v>2629088</v>
-      </c>
-      <c r="C3">
-        <f>Costos!C5</f>
-        <v>4144550</v>
-      </c>
-      <c r="G3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="17">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4">
-        <f>B2-B3</f>
-        <v>49712</v>
-      </c>
-      <c r="C4">
-        <f>C2-C3</f>
-        <v>1794250</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5">
-        <f>-(B4*H3)</f>
-        <v>-17399.199999999997</v>
-      </c>
-      <c r="C5">
-        <f>-(C4*H3)</f>
-        <v>-627987.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6">
-        <f>SUM(B4:B5)</f>
-        <v>32312.800000000003</v>
-      </c>
-      <c r="C6">
-        <f>SUM(C4:C5)</f>
-        <v>1166262.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2">
-        <v>2086920</v>
-      </c>
-      <c r="C2">
-        <f>B2+(B2*'Precios '!G3)+503577</f>
-        <v>3425265</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3">
-        <v>420000</v>
-      </c>
-      <c r="C3">
-        <f>B3+(B3*'Precios '!G4)+128250</f>
-        <v>548250</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4">
-        <v>122168</v>
-      </c>
-      <c r="C4">
-        <v>171035</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="22">
-        <f>SUM(B2:B4)</f>
-        <v>2629088</v>
-      </c>
-      <c r="C5" s="22">
-        <f>SUM(C2:C4)</f>
-        <v>4144550</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I20"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>-342853</v>
-      </c>
-      <c r="C3">
-        <f>Ganancias!B6</f>
-        <v>32312.800000000003</v>
-      </c>
-      <c r="D3">
-        <f>Ganancias!C6-Ganancias!C6*0.4</f>
-        <v>699757.5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4" s="24">
-        <v>0.23400000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="23">
-        <f>NPV(I4,C3:D3)+B3</f>
-        <v>142865.98268665507</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="24">
-        <f>IRR(B3:D3)</f>
-        <v>0.4765305007983307</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14">
-        <f>B3</f>
-        <v>-342853</v>
-      </c>
-      <c r="C14">
-        <f>B14+C3</f>
-        <v>-310540.2</v>
-      </c>
-      <c r="D14">
-        <f>C14+D3</f>
-        <v>389217.3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <f>D3</f>
-        <v>699757.5</v>
-      </c>
-      <c r="C17">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <f>-(C14)</f>
-        <v>310540.2</v>
-      </c>
-      <c r="C18">
-        <f>(B18*C17)/B17</f>
-        <v>5.3253911533638441</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1439,7 +1030,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
@@ -1457,31 +1048,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1622,4 +1213,496 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+    </row>
+    <row r="2" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="19">
+        <f>6*'01-Tipo Ingreso'!B2*'02-Volumenes Ingresos'!B4</f>
+        <v>819000</v>
+      </c>
+      <c r="C3" s="19">
+        <f>6*'01-Tipo Ingreso'!B3*'02-Volumenes Ingresos'!C4</f>
+        <v>180000</v>
+      </c>
+      <c r="D3" s="19">
+        <f>'01-Tipo Ingreso'!B4*'02-Volumenes Ingresos'!D4</f>
+        <v>10000</v>
+      </c>
+      <c r="E3" s="19">
+        <f>(('01-Tipo Ingreso'!E4*'01-Tipo Ingreso'!B5)+('01-Tipo Ingreso'!B6*'02-Volumenes Ingresos'!F4)+('01-Tipo Ingreso'!B7*'02-Volumenes Ingresos'!G4)+('01-Tipo Ingreso'!B8*'02-Volumenes Ingresos'!H4))*6</f>
+        <v>213000</v>
+      </c>
+      <c r="F3" s="19">
+        <f>SUM(B3:E3)</f>
+        <v>1222000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="19">
+        <f>6*'01-Tipo Ingreso'!B2*'02-Volumenes Ingresos'!B5</f>
+        <v>630000</v>
+      </c>
+      <c r="C4" s="19">
+        <f>6*'01-Tipo Ingreso'!B3*'02-Volumenes Ingresos'!C5</f>
+        <v>450000</v>
+      </c>
+      <c r="D4" s="19">
+        <f>'01-Tipo Ingreso'!B4*'02-Volumenes Ingresos'!D5</f>
+        <v>30000</v>
+      </c>
+      <c r="E4" s="19">
+        <f>(('01-Tipo Ingreso'!E4*'01-Tipo Ingreso'!B6)+('01-Tipo Ingreso'!B6*'02-Volumenes Ingresos'!F5)+('01-Tipo Ingreso'!B7*'02-Volumenes Ingresos'!G5)+('01-Tipo Ingreso'!B8*'02-Volumenes Ingresos'!H5))*6</f>
+        <v>346800</v>
+      </c>
+      <c r="F4" s="19">
+        <f>SUM(B4:E4)</f>
+        <v>1456800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="8">
+        <f>6*'02-Volumenes Ingresos'!B6*'01-Tipo Ingreso'!B11</f>
+        <v>1146600</v>
+      </c>
+      <c r="C5" s="8">
+        <f>'01-Tipo Ingreso'!B12*'02-Volumenes Ingresos'!C6*6</f>
+        <v>882000</v>
+      </c>
+      <c r="D5" s="8">
+        <f>'01-Tipo Ingreso'!B13*'02-Volumenes Ingresos'!D6</f>
+        <v>56000</v>
+      </c>
+      <c r="E5" s="8">
+        <f>(('01-Tipo Ingreso'!B14*'02-Volumenes Ingresos'!E6)+('01-Tipo Ingreso'!B15*'02-Volumenes Ingresos'!F6)+('01-Tipo Ingreso'!B16*'02-Volumenes Ingresos'!G6)+('01-Tipo Ingreso'!B17*'02-Volumenes Ingresos'!H6))*6</f>
+        <v>473760</v>
+      </c>
+      <c r="F5" s="9">
+        <f>SUM(B5:E5)</f>
+        <v>2558360</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="8">
+        <f>6*'01-Tipo Ingreso'!B11*'02-Volumenes Ingresos'!B7</f>
+        <v>1852200</v>
+      </c>
+      <c r="C6" s="8">
+        <f>'01-Tipo Ingreso'!B12*'02-Volumenes Ingresos'!C7*6</f>
+        <v>1134000</v>
+      </c>
+      <c r="D6" s="8">
+        <f>'01-Tipo Ingreso'!B13*'02-Volumenes Ingresos'!D7</f>
+        <v>28000</v>
+      </c>
+      <c r="E6" s="8">
+        <f>(('01-Tipo Ingreso'!B14*'02-Volumenes Ingresos'!E7)+('01-Tipo Ingreso'!B15*'02-Volumenes Ingresos'!F7)+('01-Tipo Ingreso'!B16*'02-Volumenes Ingresos'!G7)+('01-Tipo Ingreso'!B17*'02-Volumenes Ingresos'!H7))*6</f>
+        <v>366240</v>
+      </c>
+      <c r="F6" s="9">
+        <f>SUM(B6:E6)</f>
+        <v>3380440</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="28">
+        <v>2016</v>
+      </c>
+      <c r="D10" s="29">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="31">
+        <f>SUM(F3:F4)</f>
+        <v>2678800</v>
+      </c>
+      <c r="D11" s="32">
+        <f>SUM(F5:F6)</f>
+        <v>5938800</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>2086920</v>
+      </c>
+      <c r="C2">
+        <f>B2+(B2*'01-Tipo Ingreso'!G3)+503577</f>
+        <v>3425265</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>420000</v>
+      </c>
+      <c r="C3">
+        <f>B3+(B3*'01-Tipo Ingreso'!G4)+128250</f>
+        <v>548250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>122168</v>
+      </c>
+      <c r="C4">
+        <v>171035</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="21">
+        <f>SUM(B2:B4)</f>
+        <v>2629088</v>
+      </c>
+      <c r="C5" s="21">
+        <f>SUM(C2:C4)</f>
+        <v>4144550</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2">
+        <f>'03-Ingresos'!C11</f>
+        <v>2678800</v>
+      </c>
+      <c r="C2">
+        <f>'03-Ingresos'!D11</f>
+        <v>5938800</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3">
+        <f>'04-Gastos'!B5</f>
+        <v>2629088</v>
+      </c>
+      <c r="C3">
+        <f>'04-Gastos'!C5</f>
+        <v>4144550</v>
+      </c>
+      <c r="G3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="17">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4">
+        <f>B2-B3</f>
+        <v>49712</v>
+      </c>
+      <c r="C4">
+        <f>C2-C3</f>
+        <v>1794250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5">
+        <f>-(B4*H3)</f>
+        <v>-17399.199999999997</v>
+      </c>
+      <c r="C5">
+        <f>-(C4*H3)</f>
+        <v>-627987.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6">
+        <f>SUM(B4:B5)</f>
+        <v>32312.800000000003</v>
+      </c>
+      <c r="C6">
+        <f>SUM(C4:C5)</f>
+        <v>1166262.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>-342853</v>
+      </c>
+      <c r="C3">
+        <f>Ganancias!B6</f>
+        <v>32312.800000000003</v>
+      </c>
+      <c r="D3">
+        <f>Ganancias!C6-Ganancias!C6*0.4</f>
+        <v>699757.5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="23">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="22">
+        <f>NPV(I4,C3:D3)+B3</f>
+        <v>142865.98268665507</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="23">
+        <f>IRR(B3:D3)</f>
+        <v>0.4765305007983307</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14">
+        <f>B3</f>
+        <v>-342853</v>
+      </c>
+      <c r="C14">
+        <f>B14+C3</f>
+        <v>-310540.2</v>
+      </c>
+      <c r="D14">
+        <f>C14+D3</f>
+        <v>389217.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f>D3</f>
+        <v>699757.5</v>
+      </c>
+      <c r="C17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f>-(C14)</f>
+        <v>310540.2</v>
+      </c>
+      <c r="C18">
+        <f>(B18*C17)/B17</f>
+        <v>5.3253911533638441</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>